<commit_message>
ReducedMana => SwallowReducedMana 로 변경
</commit_message>
<xml_diff>
--- a/Assets/ERang/Excels/AbilityData.xlsx
+++ b/Assets/ERang/Excels/AbilityData.xlsx
@@ -437,23 +437,23 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
+    <t>Active</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>ChainAbilityId</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>삼킨 카드 비용 감소</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
     <t>Swallow</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>Active</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>ChainAbilityId</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>삼킨 카드 비용 감소</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">ReducedMana </t>
+    <t xml:space="preserve">SwallowReducedMana </t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
@@ -987,7 +987,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F50" sqref="F50"/>
+      <selection pane="bottomLeft" activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="16.5"/>
@@ -1058,7 +1058,7 @@
         <v>92</v>
       </c>
       <c r="Q1" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:17">
@@ -2581,14 +2581,14 @@
         <v>130</v>
       </c>
       <c r="C44" s="15" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="D44" s="7">
         <v>1</v>
       </c>
       <c r="E44" s="7"/>
       <c r="F44" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G44" s="7">
         <v>1</v>
@@ -2615,7 +2615,7 @@
         <v>100027</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C45" s="15" t="s">
         <v>135</v>

</xml_diff>